<commit_message>
bổ xung mấy tính năng nựa
</commit_message>
<xml_diff>
--- a/dic.xlsx
+++ b/dic.xlsx
@@ -1,14 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21617"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21722"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14238B0C-272B-4B0F-8CFA-52225E14B64F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B402A874-CB6A-4CB3-A3DF-C9351AEE88BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15225" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="753" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="0" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="2" r:id="rId2"/>
+    <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="3" sheetId="4" r:id="rId4"/>
+    <sheet name="4" sheetId="5" r:id="rId5"/>
+    <sheet name="5" sheetId="6" r:id="rId6"/>
+    <sheet name="6" sheetId="7" r:id="rId7"/>
+    <sheet name="7" sheetId="8" r:id="rId8"/>
+    <sheet name="8" sheetId="9" r:id="rId9"/>
+    <sheet name="9" sheetId="10" r:id="rId10"/>
+    <sheet name="10" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -520,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -546,7 +556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -562,7 +572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -570,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -602,7 +612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -618,7 +628,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -626,7 +636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -634,7 +644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -642,7 +652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -650,7 +660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -666,7 +676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -698,7 +708,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -706,7 +716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -714,7 +724,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -722,7 +732,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -730,7 +740,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -746,7 +756,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
@@ -757,4 +767,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF769CF-2C7C-4C75-A61B-54FB7E7E22CC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22402A94-3C10-44FE-96F0-FB1DDFA8D82A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C78893B-8F93-4315-AD36-E5DC6FF01751}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F774D74-14CB-45AB-8DB0-BC1196694758}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A11471E-D7DA-40A7-ACDC-4EB93992CE88}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E67B5C-497C-4760-8C72-0035398C0B0C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C080BFD6-026A-4BA5-B225-29217EA4A42F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51C244-1170-4CDF-AC4F-3E67D3B7947B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30673079-284C-442F-9AF0-CE7E7D36BFAB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE84361A-46C5-4557-966C-8F6A2C675675}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>